<commit_message>
Correct open_economy_export_tax data and convert it to long format
</commit_message>
<xml_diff>
--- a/library/data/SAMdata_open_economy_export_tax_matrix_format.xlsx
+++ b/library/data/SAMdata_open_economy_export_tax_matrix_format.xlsx
@@ -548,6 +548,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,8 +595,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,7 +903,7 @@
       <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,51 +941,51 @@
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="38" t="s">
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="38" t="s">
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="38" t="s">
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="39"/>
-      <c r="AE4" s="39"/>
-      <c r="AF4" s="39"/>
-      <c r="AG4" s="39"/>
-      <c r="AH4" s="39"/>
-      <c r="AI4" s="40"/>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="41"/>
+      <c r="AI4" s="42"/>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1081,10 +1081,10 @@
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1183,10 +1183,10 @@
       <c r="B7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1282,7 +1282,7 @@
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -1394,7 +1394,7 @@
       <c r="AP8" s="31"/>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1504,7 +1504,7 @@
       <c r="AP9" s="31"/>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="AP10" s="31"/>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1724,7 +1724,7 @@
       <c r="AP11" s="31"/>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1834,7 +1834,7 @@
       <c r="AP12" s="31"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1944,7 +1944,7 @@
       <c r="AP13" s="31"/>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -2054,7 +2054,7 @@
       <c r="AP14" s="31"/>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -2165,7 +2165,7 @@
       <c r="AP15" s="31"/>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -2275,7 +2275,7 @@
       <c r="AN16" s="31"/>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
@@ -2383,7 +2383,7 @@
       <c r="AN17" s="31"/>
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="AN18" s="31"/>
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="AN19" s="31"/>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2707,7 +2707,7 @@
       <c r="AN20" s="31"/>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -2815,7 +2815,7 @@
       <c r="AN21" s="31"/>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
@@ -2923,7 +2923,7 @@
       <c r="AN22" s="31"/>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
@@ -3031,7 +3031,7 @@
       <c r="AN23" s="31"/>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="45" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -3068,16 +3068,16 @@
         <v>0</v>
       </c>
       <c r="M24" s="9">
-        <v>6815.6899538995031</v>
+        <v>6819.8609177240432</v>
       </c>
       <c r="N24" s="9">
-        <v>77966.424644897619</v>
+        <v>78067.900786550003</v>
       </c>
       <c r="O24" s="9">
-        <v>17340.797086666065</v>
+        <v>17347.834397631777</v>
       </c>
       <c r="P24" s="9">
-        <v>280618.54387689277</v>
+        <v>280716.15635398572</v>
       </c>
       <c r="Q24" s="9">
         <v>178.71</v>
@@ -3116,13 +3116,13 @@
         <v>0</v>
       </c>
       <c r="AC24" s="9">
-        <v>815075.51326772675</v>
+        <v>815277.07297017646</v>
       </c>
       <c r="AD24" s="9">
         <v>0</v>
       </c>
       <c r="AE24" s="9">
-        <v>211726.20669264629</v>
+        <v>211795.29570805206</v>
       </c>
       <c r="AF24" s="9">
         <v>5467.680444395216</v>
@@ -3141,7 +3141,7 @@
       <c r="AN24" s="31"/>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="3" t="s">
         <v>2</v>
       </c>
@@ -3249,7 +3249,7 @@
       <c r="AN25" s="31"/>
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -3357,7 +3357,7 @@
       <c r="AN26" s="31"/>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
@@ -3392,16 +3392,16 @@
         <v>0</v>
       </c>
       <c r="M27" s="9">
-        <v>163852.30207031738</v>
+        <v>163848.13110649283</v>
       </c>
       <c r="N27" s="9">
-        <v>1032581.5749182442</v>
+        <v>1032480.0987765919</v>
       </c>
       <c r="O27" s="9">
-        <v>353900.29007247643</v>
+        <v>353893.2527615109</v>
       </c>
       <c r="P27" s="9">
-        <v>3328299.2658602078</v>
+        <v>3328201.6533831153</v>
       </c>
       <c r="Q27" s="9">
         <v>0</v>
@@ -3465,7 +3465,7 @@
       <c r="AN27" s="31"/>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -3551,10 +3551,10 @@
         <v>1933.2814019793727</v>
       </c>
       <c r="AD28" s="30">
-        <v>1933.2814019793727</v>
+        <v>190.88246438291412</v>
       </c>
       <c r="AE28" s="30">
-        <v>1933.2814019793727</v>
+        <v>532.04571966391779</v>
       </c>
       <c r="AF28" s="9">
         <v>0</v>
@@ -3573,7 +3573,7 @@
       <c r="AN28" s="31"/>
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
@@ -3681,7 +3681,7 @@
       <c r="AN29" s="31"/>
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="AN30" s="31"/>
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
@@ -3897,7 +3897,7 @@
       <c r="AN31" s="31"/>
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="47" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="X32" s="9">
         <f>SUM(M27:P27)</f>
-        <v>4878633.4329212457</v>
+        <v>4878423.1360277105</v>
       </c>
       <c r="Y32" s="9">
         <v>0</v>
@@ -3993,7 +3993,7 @@
         <v>0</v>
       </c>
       <c r="AF32" s="30">
-        <v>100000</v>
+        <v>96856.365380087867</v>
       </c>
       <c r="AG32" s="30">
         <v>0</v>
@@ -4013,7 +4013,7 @@
       <c r="AP32" s="17"/>
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -4073,7 +4073,7 @@
       </c>
       <c r="U33" s="9">
         <f>SUM(M24:T24)+SUM(AC24:AI24)</f>
-        <v>1465180.6913873011</v>
+        <v>1465661.6369986923</v>
       </c>
       <c r="V33" s="9">
         <v>0</v>
@@ -4098,7 +4098,7 @@
         <v>0</v>
       </c>
       <c r="AC33" s="30">
-        <v>1310461.3520444911</v>
+        <v>1308238.0074955034</v>
       </c>
       <c r="AD33" s="30">
         <v>0</v>
@@ -4126,7 +4126,7 @@
       <c r="AP33" s="17"/>
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>0</v>
       </c>
       <c r="AC34" s="30">
-        <v>2590414.0752308122</v>
+        <v>2589081.9285639026</v>
       </c>
       <c r="AD34" s="30">
         <v>0</v>
@@ -4237,7 +4237,7 @@
       <c r="AP34" s="17"/>
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="3" t="s">
         <v>11</v>
       </c>
@@ -4351,7 +4351,7 @@
       <c r="AP35" s="17"/>
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="Y36" s="9">
         <f>SUM(M28:T28)+SUM(AC28:AI28)</f>
-        <v>129953.17547229752</v>
+        <v>126809.5408523856</v>
       </c>
       <c r="Z36" s="9">
         <v>0</v>
@@ -4445,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="AF36" s="30">
-        <v>1711609.54427642</v>
+        <v>1714753.1788963322</v>
       </c>
       <c r="AG36" s="30">
         <v>0</v>
@@ -4465,7 +4465,7 @@
       <c r="AP36" s="17"/>
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
@@ -4576,7 +4576,7 @@
       <c r="AP37" s="17"/>
     </row>
     <row r="38" spans="1:43" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
+      <c r="A38" s="48"/>
       <c r="B38" s="3" t="s">
         <v>28</v>
       </c>
@@ -4687,7 +4687,7 @@
       <c r="AP38" s="31"/>
     </row>
     <row r="39" spans="1:43" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="3" t="s">
         <v>28</v>
       </c>
@@ -4798,7 +4798,7 @@
       <c r="AP39" s="31"/>
     </row>
     <row r="40" spans="1:43" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="3" t="s">
         <v>28</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="AP40" s="31"/>
     </row>
     <row r="41" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
+      <c r="A41" s="49"/>
       <c r="B41" s="3" t="s">
         <v>28</v>
       </c>
@@ -5095,6 +5095,25 @@
       <c r="AF45" s="17"/>
     </row>
     <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
+      <c r="S46" s="31"/>
+      <c r="T46" s="31"/>
+      <c r="U46" s="31"/>
+      <c r="V46" s="31"/>
+      <c r="W46" s="31"/>
+      <c r="X46" s="31"/>
+      <c r="Y46" s="31"/>
+      <c r="Z46" s="31"/>
+      <c r="AA46" s="31"/>
+      <c r="AB46" s="31"/>
+      <c r="AC46" s="31"/>
+      <c r="AD46" s="31"/>
+      <c r="AE46" s="31"/>
       <c r="AF46" s="31"/>
       <c r="AI46" s="33"/>
       <c r="AJ46" s="33"/>
@@ -5131,8 +5150,9 @@
       <c r="AQ48" s="35"/>
     </row>
     <row r="49" spans="13:43" x14ac:dyDescent="0.25">
-      <c r="AD49" s="29"/>
-      <c r="AE49" s="29"/>
+      <c r="AC49" s="31"/>
+      <c r="AD49" s="31"/>
+      <c r="AE49" s="31"/>
       <c r="AF49" s="29"/>
       <c r="AG49" s="29"/>
       <c r="AH49" s="29"/>
@@ -5463,51 +5483,51 @@
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="38" t="s">
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="38" t="s">
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="38" t="s">
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="39"/>
-      <c r="AE4" s="39"/>
-      <c r="AF4" s="39"/>
-      <c r="AG4" s="39"/>
-      <c r="AH4" s="39"/>
-      <c r="AI4" s="40"/>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="41"/>
+      <c r="AI4" s="42"/>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
@@ -5603,10 +5623,10 @@
       </c>
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
@@ -5705,10 +5725,10 @@
       <c r="B7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
@@ -5804,7 +5824,7 @@
       </c>
     </row>
     <row r="8" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -5915,7 +5935,7 @@
       <c r="AN8" s="31"/>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
@@ -6027,7 +6047,7 @@
       <c r="AU9" s="29"/>
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -6139,7 +6159,7 @@
       <c r="AU10" s="29"/>
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -6251,7 +6271,7 @@
       <c r="AU11" s="29"/>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -6286,16 +6306,16 @@
         <v>0</v>
       </c>
       <c r="M12" s="9">
-        <v>16.965130702967375</v>
+        <v>17.64373593108607</v>
       </c>
       <c r="N12" s="12">
-        <v>37.291197181804208</v>
+        <v>38.782845069076373</v>
       </c>
       <c r="O12" s="12">
-        <v>0.43483103569046533</v>
+        <v>0.45222427711808399</v>
       </c>
       <c r="P12" s="12">
-        <v>21.012244816387241</v>
+        <v>21.852734609042731</v>
       </c>
       <c r="Q12" s="11">
         <v>0</v>
@@ -6334,13 +6354,13 @@
         <v>0</v>
       </c>
       <c r="AC12" s="12">
-        <v>250.97521489644751</v>
+        <v>261.01422349230546</v>
       </c>
       <c r="AD12" s="12">
         <v>0</v>
       </c>
       <c r="AE12" s="12">
-        <v>27.206038740824212</v>
+        <v>28.294280290457181</v>
       </c>
       <c r="AF12" s="11">
         <v>0</v>
@@ -6363,7 +6383,7 @@
       <c r="AU12" s="29"/>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -6398,16 +6418,16 @@
         <v>0</v>
       </c>
       <c r="M13" s="9">
-        <v>164.71182214000692</v>
+        <v>166.35894036140698</v>
       </c>
       <c r="N13" s="12">
-        <v>5735.5487692742126</v>
+        <v>5792.9042569669546</v>
       </c>
       <c r="O13" s="12">
-        <v>364.59853660114896</v>
+        <v>368.24452196716049</v>
       </c>
       <c r="P13" s="12">
-        <v>4557.8925025391973</v>
+        <v>4603.4714275645883</v>
       </c>
       <c r="Q13" s="11">
         <v>0</v>
@@ -6446,13 +6466,13 @@
         <v>0</v>
       </c>
       <c r="AC13" s="12">
-        <v>15791.191311471635</v>
+        <v>15949.103224586352</v>
       </c>
       <c r="AD13" s="12">
         <v>0</v>
       </c>
       <c r="AE13" s="12">
-        <v>6570.8333002596337</v>
+        <v>6636.5416332622299</v>
       </c>
       <c r="AF13" s="11">
         <v>0</v>
@@ -6475,7 +6495,7 @@
       <c r="AU13" s="29"/>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -6558,13 +6578,13 @@
         <v>0</v>
       </c>
       <c r="AC14" s="12">
-        <v>2.8054317691335942E-2</v>
+        <v>3.0018119929729453E-2</v>
       </c>
       <c r="AD14" s="12">
         <v>0</v>
       </c>
       <c r="AE14" s="12">
-        <v>0.55603854321171253</v>
+        <v>0.59496124123653227</v>
       </c>
       <c r="AF14" s="11">
         <v>0</v>
@@ -6587,7 +6607,7 @@
       <c r="AU14" s="29"/>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -6622,16 +6642,16 @@
         <v>0</v>
       </c>
       <c r="M15" s="9">
-        <v>92.262018751066378</v>
+        <v>94.107259126087726</v>
       </c>
       <c r="N15" s="12">
-        <v>2131.45030361923</v>
+        <v>2174.079309691615</v>
       </c>
       <c r="O15" s="12">
-        <v>168.69661791373079</v>
+        <v>172.07055027200545</v>
       </c>
       <c r="P15" s="12">
-        <v>2559.6531137473921</v>
+        <v>2610.8461760223399</v>
       </c>
       <c r="Q15" s="11">
         <v>0</v>
@@ -6670,13 +6690,13 @@
         <v>0</v>
       </c>
       <c r="AC15" s="12">
-        <v>1680.3408468449684</v>
+        <v>1713.9476637818677</v>
       </c>
       <c r="AD15" s="12">
         <v>0</v>
       </c>
       <c r="AE15" s="12">
-        <v>112.67590777366559</v>
+        <v>114.92942592913889</v>
       </c>
       <c r="AF15" s="11">
         <v>0</v>
@@ -6700,7 +6720,7 @@
       <c r="AU15" s="29"/>
     </row>
     <row r="16" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -6811,7 +6831,7 @@
       <c r="AN16" s="31"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
@@ -6920,7 +6940,7 @@
       <c r="AN17" s="31"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
@@ -7029,7 +7049,7 @@
       <c r="AN18" s="31"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -7138,7 +7158,7 @@
       <c r="AN19" s="31"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -7247,7 +7267,7 @@
       <c r="AN20" s="31"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -7356,7 +7376,7 @@
       <c r="AN21" s="31"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
@@ -7465,7 +7485,7 @@
       <c r="AN22" s="31"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
@@ -7574,7 +7594,7 @@
       <c r="AN23" s="31"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="45" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -7599,28 +7619,28 @@
         <v>818112.77519823459</v>
       </c>
       <c r="I24" s="18">
-        <v>353.88465737412099</v>
+        <v>368.04004366908589</v>
       </c>
       <c r="J24" s="18">
-        <v>33184.776242285836</v>
+        <v>33516.62400470869</v>
       </c>
       <c r="K24" s="18">
-        <v>0.58409286090304846</v>
+        <v>0.62497936116626174</v>
       </c>
       <c r="L24" s="18">
-        <v>6745.0788086500543</v>
+        <v>6879.9803848230549</v>
       </c>
       <c r="M24" s="9">
-        <v>-6815.6899538995031</v>
+        <v>-6819.8609177240432</v>
       </c>
       <c r="N24" s="12">
-        <v>-77966.424644897619</v>
+        <v>-78067.900786550003</v>
       </c>
       <c r="O24" s="12">
-        <v>-17340.797086666065</v>
+        <v>-17347.834397631777</v>
       </c>
       <c r="P24" s="12">
-        <v>-280618.54387689277</v>
+        <v>-280716.15635398572</v>
       </c>
       <c r="Q24" s="12">
         <v>0</v>
@@ -7659,13 +7679,13 @@
         <v>0</v>
       </c>
       <c r="AC24" s="12">
-        <v>-815075.51326772675</v>
+        <v>-815277.07297017646</v>
       </c>
       <c r="AD24" s="12">
         <v>0</v>
       </c>
       <c r="AE24" s="12">
-        <v>-211726.20669264629</v>
+        <v>-211795.29570805206</v>
       </c>
       <c r="AF24" s="12">
         <v>0</v>
@@ -7685,7 +7705,7 @@
       <c r="AN24" s="31"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="3" t="s">
         <v>2</v>
       </c>
@@ -7794,7 +7814,7 @@
       <c r="AN25" s="31"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -7903,7 +7923,7 @@
       <c r="AN26" s="31"/>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
@@ -8012,7 +8032,7 @@
       <c r="AN27" s="31"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -8121,7 +8141,7 @@
       <c r="AN28" s="31"/>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
@@ -8230,7 +8250,7 @@
       <c r="AN29" s="31"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
@@ -8339,7 +8359,7 @@
       <c r="AN30" s="31"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
@@ -8448,7 +8468,7 @@
       <c r="AN31" s="31"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="47" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -8559,7 +8579,7 @@
       <c r="AN32" s="31"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -8668,7 +8688,7 @@
       <c r="AN33" s="31"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -8777,7 +8797,7 @@
       <c r="AN34" s="31"/>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="3" t="s">
         <v>11</v>
       </c>
@@ -8886,7 +8906,7 @@
       <c r="AN35" s="31"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -8995,7 +9015,7 @@
       <c r="AN36" s="31"/>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
@@ -9104,7 +9124,7 @@
       <c r="AN37" s="31"/>
     </row>
     <row r="38" spans="1:40" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
+      <c r="A38" s="48"/>
       <c r="B38" s="3" t="s">
         <v>28</v>
       </c>
@@ -9213,7 +9233,7 @@
       <c r="AN38" s="31"/>
     </row>
     <row r="39" spans="1:40" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="3" t="s">
         <v>28</v>
       </c>
@@ -9322,7 +9342,7 @@
       <c r="AN39" s="31"/>
     </row>
     <row r="40" spans="1:40" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="3" t="s">
         <v>28</v>
       </c>
@@ -9431,7 +9451,7 @@
       <c r="AN40" s="31"/>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
+      <c r="A41" s="49"/>
       <c r="B41" s="3" t="s">
         <v>28</v>
       </c>
@@ -9541,11 +9561,11 @@
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D42" s="37"/>
-      <c r="E42" s="54"/>
+      <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
       <c r="I43" s="31"/>
@@ -9577,43 +9597,55 @@
       <c r="AI43" s="31"/>
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="E44" s="53"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="31"/>
-      <c r="M44" s="31"/>
-      <c r="N44" s="31"/>
-      <c r="O44" s="31"/>
-      <c r="P44" s="31"/>
-      <c r="Q44" s="31"/>
-      <c r="R44" s="31"/>
-      <c r="S44" s="31"/>
-      <c r="T44" s="31"/>
-      <c r="U44" s="31"/>
-      <c r="V44" s="31"/>
-      <c r="W44" s="31"/>
-      <c r="X44" s="31"/>
-      <c r="Y44" s="31"/>
-      <c r="Z44" s="31"/>
-      <c r="AA44" s="31"/>
-      <c r="AB44" s="31"/>
-      <c r="AC44" s="31"/>
-      <c r="AD44" s="31"/>
-      <c r="AE44" s="31"/>
-      <c r="AF44" s="31"/>
-      <c r="AG44" s="31"/>
-      <c r="AH44" s="31"/>
-      <c r="AI44" s="31"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="38"/>
+      <c r="S44" s="38"/>
+      <c r="T44" s="38"/>
+      <c r="U44" s="38"/>
+      <c r="V44" s="38"/>
+      <c r="W44" s="38"/>
+      <c r="X44" s="38"/>
+      <c r="Y44" s="38"/>
+      <c r="Z44" s="38"/>
+      <c r="AA44" s="38"/>
+      <c r="AB44" s="38"/>
+      <c r="AC44" s="38"/>
+      <c r="AD44" s="38"/>
+      <c r="AE44" s="38"/>
+      <c r="AF44" s="38"/>
+      <c r="AG44" s="38"/>
+      <c r="AH44" s="38"/>
+      <c r="AI44" s="38"/>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="N45" s="29"/>
+      <c r="O45" s="29"/>
+      <c r="P45" s="29"/>
+      <c r="Q45" s="29"/>
+      <c r="R45" s="29"/>
+      <c r="S45" s="29"/>
+      <c r="T45" s="29"/>
+      <c r="AC45" s="29"/>
       <c r="AD45" s="29"/>
       <c r="AE45" s="29"/>
+      <c r="AF45" s="29"/>
+      <c r="AG45" s="29"/>
+      <c r="AH45" s="29"/>
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="M46" s="29"/>
       <c r="N46" s="29"/>
       <c r="O46" s="29"/>
       <c r="P46" s="29"/>
@@ -9621,19 +9653,19 @@
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
       <c r="T46" s="29"/>
-      <c r="AC46" s="31"/>
-      <c r="AD46" s="31"/>
-      <c r="AE46" s="31"/>
+      <c r="AC46" s="29"/>
+      <c r="AD46" s="29"/>
+      <c r="AE46" s="29"/>
       <c r="AF46" s="29"/>
       <c r="AG46" s="29"/>
       <c r="AH46" s="29"/>
       <c r="AI46" s="29"/>
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="31"/>
-      <c r="P47" s="31"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
@@ -9672,19 +9704,19 @@
       <c r="R49" s="29"/>
       <c r="S49" s="29"/>
       <c r="T49" s="29"/>
-      <c r="AC49" s="31"/>
-      <c r="AD49" s="31"/>
-      <c r="AE49" s="31"/>
+      <c r="AC49" s="29"/>
+      <c r="AD49" s="29"/>
+      <c r="AE49" s="29"/>
       <c r="AF49" s="29"/>
       <c r="AG49" s="29"/>
       <c r="AH49" s="29"/>
       <c r="AI49" s="29"/>
     </row>
     <row r="50" spans="13:36" x14ac:dyDescent="0.25">
-      <c r="M50" s="31"/>
-      <c r="N50" s="31"/>
-      <c r="O50" s="31"/>
-      <c r="P50" s="31"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
       <c r="Q50" s="29"/>
       <c r="R50" s="29"/>
       <c r="S50" s="29"/>
@@ -9775,11 +9807,16 @@
       <c r="AE55" s="29"/>
     </row>
     <row r="56" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="M56" s="29"/>
+      <c r="N56" s="29"/>
+      <c r="O56" s="29"/>
+      <c r="P56" s="29"/>
       <c r="AC56" s="29"/>
       <c r="AD56" s="29"/>
       <c r="AE56" s="29"/>
     </row>
     <row r="57" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="M57" s="29"/>
       <c r="N57" s="29"/>
       <c r="O57" s="29"/>
       <c r="P57" s="29"/>
@@ -9852,17 +9889,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="A16:A23"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A32:A41"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E4:L4"/>
     <mergeCell ref="M4:T4"/>
     <mergeCell ref="U4:AB4"/>
     <mergeCell ref="AC4:AI4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="A16:A23"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A32:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -9918,51 +9955,51 @@
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="38" t="s">
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="38" t="s">
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="38" t="s">
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="39"/>
-      <c r="AE4" s="39"/>
-      <c r="AF4" s="39"/>
-      <c r="AG4" s="39"/>
-      <c r="AH4" s="39"/>
-      <c r="AI4" s="40"/>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="41"/>
+      <c r="AI4" s="42"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
@@ -10058,10 +10095,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
@@ -10160,10 +10197,10 @@
       <c r="B7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
@@ -10259,7 +10296,7 @@
       </c>
     </row>
     <row r="8" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -10370,7 +10407,7 @@
       <c r="AN8" s="31"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
@@ -10479,7 +10516,7 @@
       <c r="AN9" s="31"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -10588,7 +10625,7 @@
       <c r="AN10" s="31"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -10697,7 +10734,7 @@
       <c r="AN11" s="31"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -10806,7 +10843,7 @@
       <c r="AN12" s="31"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -10915,7 +10952,7 @@
       <c r="AN13" s="31"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -11024,7 +11061,7 @@
       <c r="AN14" s="31"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -11134,7 +11171,7 @@
       <c r="AN15" s="31"/>
     </row>
     <row r="16" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -11245,7 +11282,7 @@
       <c r="AN16" s="31"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
@@ -11354,7 +11391,7 @@
       <c r="AN17" s="31"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
@@ -11463,7 +11500,7 @@
       <c r="AN18" s="31"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -11572,7 +11609,7 @@
       <c r="AN19" s="31"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -11681,7 +11718,7 @@
       <c r="AN20" s="31"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -11790,7 +11827,7 @@
       <c r="AN21" s="31"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
@@ -11899,7 +11936,7 @@
       <c r="AN22" s="31"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
@@ -12008,7 +12045,7 @@
       <c r="AN23" s="31"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="45" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -12119,7 +12156,7 @@
       <c r="AN24" s="31"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="3" t="s">
         <v>2</v>
       </c>
@@ -12228,7 +12265,7 @@
       <c r="AN25" s="31"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -12337,7 +12374,7 @@
       <c r="AN26" s="31"/>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
@@ -12446,7 +12483,7 @@
       <c r="AN27" s="31"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -12555,7 +12592,7 @@
       <c r="AN28" s="31"/>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
@@ -12664,7 +12701,7 @@
       <c r="AN29" s="31"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
@@ -12773,7 +12810,7 @@
       <c r="AN30" s="31"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
@@ -12882,7 +12919,7 @@
       <c r="AN31" s="31"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="47" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -12993,7 +13030,7 @@
       <c r="AN32" s="31"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -13102,7 +13139,7 @@
       <c r="AN33" s="31"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -13211,7 +13248,7 @@
       <c r="AN34" s="31"/>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="3" t="s">
         <v>11</v>
       </c>
@@ -13320,7 +13357,7 @@
       <c r="AN35" s="31"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -13429,7 +13466,7 @@
       <c r="AN36" s="31"/>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
@@ -13538,7 +13575,7 @@
       <c r="AN37" s="31"/>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
+      <c r="A38" s="48"/>
       <c r="B38" s="3" t="s">
         <v>28</v>
       </c>
@@ -13647,7 +13684,7 @@
       <c r="AN38" s="31"/>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="3" t="s">
         <v>28</v>
       </c>
@@ -13756,7 +13793,7 @@
       <c r="AN39" s="31"/>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="3" t="s">
         <v>28</v>
       </c>
@@ -13865,7 +13902,7 @@
       <c r="AN40" s="31"/>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
+      <c r="A41" s="49"/>
       <c r="B41" s="3" t="s">
         <v>28</v>
       </c>
@@ -13975,10 +14012,10 @@
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="D42" s="37"/>
-      <c r="E42" s="54"/>
+      <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E43" s="53"/>
+      <c r="E43" s="38"/>
       <c r="F43" s="31"/>
       <c r="G43" s="31"/>
       <c r="H43" s="31"/>
@@ -14067,17 +14104,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E4:L4"/>
+    <mergeCell ref="M4:T4"/>
+    <mergeCell ref="U4:AB4"/>
+    <mergeCell ref="AC4:AI4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A8:A15"/>
     <mergeCell ref="A16:A23"/>
     <mergeCell ref="A24:A31"/>
     <mergeCell ref="A32:A41"/>
-    <mergeCell ref="E4:L4"/>
-    <mergeCell ref="M4:T4"/>
-    <mergeCell ref="U4:AB4"/>
-    <mergeCell ref="AC4:AI4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -14092,7 +14129,7 @@
       <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14127,51 +14164,51 @@
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="38" t="s">
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="38" t="s">
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="38" t="s">
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="39"/>
-      <c r="AE4" s="39"/>
-      <c r="AF4" s="39"/>
-      <c r="AG4" s="39"/>
-      <c r="AH4" s="39"/>
-      <c r="AI4" s="40"/>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="41"/>
+      <c r="AI4" s="42"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
@@ -14267,10 +14304,10 @@
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
@@ -14369,10 +14406,10 @@
       <c r="B7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
@@ -14468,7 +14505,7 @@
       </c>
     </row>
     <row r="8" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -14609,7 +14646,7 @@
       <c r="AN8" s="31"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
@@ -14748,7 +14785,7 @@
       <c r="AN9" s="31"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -14887,7 +14924,7 @@
       <c r="AN10" s="31"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -15026,7 +15063,7 @@
       <c r="AN11" s="31"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -15070,19 +15107,19 @@
       </c>
       <c r="M12" s="9">
         <f>basic_price!M12+tax_layer!M12+export_tax!M12</f>
-        <v>1623.7784023275619</v>
+        <v>1624.4570075556805</v>
       </c>
       <c r="N12" s="12">
         <f>basic_price!N12+tax_layer!N12+export_tax!N12</f>
-        <v>10004.594067120983</v>
+        <v>10006.085715008254</v>
       </c>
       <c r="O12" s="12">
         <f>basic_price!O12+tax_layer!O12+export_tax!O12</f>
-        <v>93.388625127595873</v>
+        <v>93.406018369023485</v>
       </c>
       <c r="P12" s="12">
         <f>basic_price!P12+tax_layer!P12+export_tax!P12</f>
-        <v>1092.4231019959614</v>
+        <v>1093.2635917886168</v>
       </c>
       <c r="Q12" s="11">
         <f>basic_price!Q12+tax_layer!Q12+export_tax!Q12</f>
@@ -15134,7 +15171,7 @@
       </c>
       <c r="AC12" s="12">
         <f>basic_price!AC12+tax_layer!AC12+export_tax!AC12</f>
-        <v>6103.3373166888969</v>
+        <v>6113.3763252847548</v>
       </c>
       <c r="AD12" s="12">
         <f>basic_price!AD12+tax_layer!AD12+export_tax!AD12</f>
@@ -15142,7 +15179,7 @@
       </c>
       <c r="AE12" s="12">
         <f>basic_price!AE12+tax_layer!AE12+export_tax!AE12</f>
-        <v>965.10130405352663</v>
+        <v>966.18954560315967</v>
       </c>
       <c r="AF12" s="11">
         <f>basic_price!AF12+tax_layer!AF12+export_tax!AF12</f>
@@ -15165,7 +15202,7 @@
       <c r="AN12" s="31"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -15209,19 +15246,19 @@
       </c>
       <c r="M13" s="9">
         <f>basic_price!M13+tax_layer!M13+export_tax!M13</f>
-        <v>4257.7342867055031</v>
+        <v>4259.3814049269031</v>
       </c>
       <c r="N13" s="12">
         <f>basic_price!N13+tax_layer!N13+export_tax!N13</f>
-        <v>332666.4608381716</v>
+        <v>332723.81632586435</v>
       </c>
       <c r="O13" s="12">
         <f>basic_price!O13+tax_layer!O13+export_tax!O13</f>
-        <v>17061.346407453952</v>
+        <v>17064.992392819964</v>
       </c>
       <c r="P13" s="12">
         <f>basic_price!P13+tax_layer!P13+export_tax!P13</f>
-        <v>66191.942200674501</v>
+        <v>66237.521125699888</v>
       </c>
       <c r="Q13" s="11">
         <f>basic_price!Q13+tax_layer!Q13+export_tax!Q13</f>
@@ -15273,7 +15310,7 @@
       </c>
       <c r="AC13" s="12">
         <f>basic_price!AC13+tax_layer!AC13+export_tax!AC13</f>
-        <v>163009.69862548498</v>
+        <v>163167.61053859969</v>
       </c>
       <c r="AD13" s="12">
         <f>basic_price!AD13+tax_layer!AD13+export_tax!AD13</f>
@@ -15281,7 +15318,7 @@
       </c>
       <c r="AE13" s="12">
         <f>basic_price!AE13+tax_layer!AE13+export_tax!AE13</f>
-        <v>53757.44806104515</v>
+        <v>53823.156394047743</v>
       </c>
       <c r="AF13" s="11">
         <f>basic_price!AF13+tax_layer!AF13+export_tax!AF13</f>
@@ -15304,7 +15341,7 @@
       <c r="AN13" s="31"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -15412,7 +15449,7 @@
       </c>
       <c r="AC14" s="12">
         <f>basic_price!AC14+tax_layer!AC14+export_tax!AC14</f>
-        <v>0.42601558569234155</v>
+        <v>0.42797938793073509</v>
       </c>
       <c r="AD14" s="12">
         <f>basic_price!AD14+tax_layer!AD14+export_tax!AD14</f>
@@ -15420,7 +15457,7 @@
       </c>
       <c r="AE14" s="12">
         <f>basic_price!AE14+tax_layer!AE14+export_tax!AE14</f>
-        <v>10.416888960186496</v>
+        <v>10.455811658211315</v>
       </c>
       <c r="AF14" s="11">
         <f>basic_price!AF14+tax_layer!AF14+export_tax!AF14</f>
@@ -15443,7 +15480,7 @@
       <c r="AN14" s="31"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -15487,19 +15524,19 @@
       </c>
       <c r="M15" s="9">
         <f>basic_price!M15+tax_layer!M15+export_tax!M15</f>
-        <v>3373.4774079932445</v>
+        <v>3375.3226483682656</v>
       </c>
       <c r="N15" s="12">
         <f>basic_price!N15+tax_layer!N15+export_tax!N15</f>
-        <v>195829.59339191261</v>
+        <v>195872.222397985</v>
       </c>
       <c r="O15" s="12">
         <f>basic_price!O15+tax_layer!O15+export_tax!O15</f>
-        <v>11958.282234733948</v>
+        <v>11961.656167092222</v>
       </c>
       <c r="P15" s="12">
         <f>basic_price!P15+tax_layer!P15+export_tax!P15</f>
-        <v>59362.473862425933</v>
+        <v>59413.666924700883</v>
       </c>
       <c r="Q15" s="11">
         <f>basic_price!Q15+tax_layer!Q15+export_tax!Q15</f>
@@ -15551,7 +15588,7 @@
       </c>
       <c r="AC15" s="12">
         <f>basic_price!AC15+tax_layer!AC15+export_tax!AC15</f>
-        <v>14458.673068302071</v>
+        <v>14492.27988523897</v>
       </c>
       <c r="AD15" s="12">
         <f>basic_price!AD15+tax_layer!AD15+export_tax!AD15</f>
@@ -15559,7 +15596,7 @@
       </c>
       <c r="AE15" s="12">
         <f>basic_price!AE15+tax_layer!AE15+export_tax!AE15</f>
-        <v>1547.4852711087703</v>
+        <v>1549.7387892642437</v>
       </c>
       <c r="AF15" s="11">
         <f>basic_price!AF15+tax_layer!AF15+export_tax!AF15</f>
@@ -15582,7 +15619,7 @@
       <c r="AN15" s="31"/>
     </row>
     <row r="16" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -15723,7 +15760,7 @@
       <c r="AN16" s="31"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
@@ -15862,7 +15899,7 @@
       <c r="AN17" s="31"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
@@ -16001,7 +16038,7 @@
       <c r="AN18" s="31"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -16140,7 +16177,7 @@
       <c r="AN19" s="31"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -16279,7 +16316,7 @@
       <c r="AN20" s="31"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -16418,7 +16455,7 @@
       <c r="AN21" s="31"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
@@ -16557,7 +16594,7 @@
       <c r="AN22" s="31"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
@@ -16696,7 +16733,7 @@
       <c r="AN23" s="31"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="45" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -16726,19 +16763,19 @@
       </c>
       <c r="I24" s="18">
         <f>basic_price!I24+tax_layer!I24+export_tax!I24</f>
-        <v>353.88465737412099</v>
+        <v>368.04004366908589</v>
       </c>
       <c r="J24" s="18">
         <f>basic_price!J24+tax_layer!J24+export_tax!J24</f>
-        <v>33184.776242285836</v>
+        <v>33516.62400470869</v>
       </c>
       <c r="K24" s="18">
         <f>basic_price!K24+tax_layer!K24+export_tax!K24</f>
-        <v>0.58409286090304846</v>
+        <v>0.62497936116626174</v>
       </c>
       <c r="L24" s="18">
         <f>basic_price!L24+tax_layer!L24+export_tax!L24</f>
-        <v>6745.0788086500543</v>
+        <v>6879.9803848230549</v>
       </c>
       <c r="M24" s="9">
         <f>basic_price!M24+tax_layer!M24+export_tax!M24</f>
@@ -16837,7 +16874,7 @@
       <c r="AN24" s="31"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="3" t="s">
         <v>2</v>
       </c>
@@ -16976,7 +17013,7 @@
       <c r="AN25" s="31"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -17115,7 +17152,7 @@
       <c r="AN26" s="31"/>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
@@ -17159,19 +17196,19 @@
       </c>
       <c r="M27" s="9">
         <f>basic_price!M27+tax_layer!M27+export_tax!M27</f>
-        <v>163852.30207031738</v>
+        <v>163848.13110649283</v>
       </c>
       <c r="N27" s="12">
         <f>basic_price!N27+tax_layer!N27+export_tax!N27</f>
-        <v>1032581.5749182442</v>
+        <v>1032480.0987765919</v>
       </c>
       <c r="O27" s="12">
         <f>basic_price!O27+tax_layer!O27+export_tax!O27</f>
-        <v>353900.29007247643</v>
+        <v>353893.2527615109</v>
       </c>
       <c r="P27" s="12">
         <f>basic_price!P27+tax_layer!P27+export_tax!P27</f>
-        <v>3328299.2658602078</v>
+        <v>3328201.6533831153</v>
       </c>
       <c r="Q27" s="18">
         <f>basic_price!Q27+tax_layer!Q27+export_tax!Q27</f>
@@ -17254,7 +17291,7 @@
       <c r="AN27" s="31"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -17366,11 +17403,11 @@
       </c>
       <c r="AD28" s="12">
         <f>basic_price!AD28+tax_layer!AD28+export_tax!AD28</f>
-        <v>1742.3989375964586</v>
+        <v>0</v>
       </c>
       <c r="AE28" s="12">
         <f>basic_price!AE28+tax_layer!AE28+export_tax!AE28</f>
-        <v>1401.2356823154551</v>
+        <v>0</v>
       </c>
       <c r="AF28" s="12">
         <f>basic_price!AF28+tax_layer!AF28+export_tax!AF28</f>
@@ -17393,7 +17430,7 @@
       <c r="AN28" s="31"/>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
@@ -17532,7 +17569,7 @@
       <c r="AN29" s="31"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
@@ -17671,7 +17708,7 @@
       <c r="AN30" s="31"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
@@ -17810,7 +17847,7 @@
       <c r="AN31" s="31"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="47" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -17900,7 +17937,7 @@
       </c>
       <c r="X32" s="12">
         <f>basic_price!X32+tax_layer!X32+export_tax!X32</f>
-        <v>4878633.4329212457</v>
+        <v>4878423.1360277105</v>
       </c>
       <c r="Y32" s="12">
         <f>basic_price!Y32+tax_layer!Y32+export_tax!Y32</f>
@@ -17932,7 +17969,7 @@
       </c>
       <c r="AF32" s="12">
         <f>basic_price!AF32+tax_layer!AF32+export_tax!AF32</f>
-        <v>100000</v>
+        <v>96856.365380087867</v>
       </c>
       <c r="AG32" s="12">
         <f>basic_price!AG32+tax_layer!AG32+export_tax!AG32</f>
@@ -17951,7 +17988,7 @@
       <c r="AN32" s="31"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -18027,7 +18064,7 @@
       </c>
       <c r="U33" s="12">
         <f>basic_price!U33+tax_layer!U33+export_tax!U33</f>
-        <v>1465180.6913873011</v>
+        <v>1465661.6369986923</v>
       </c>
       <c r="V33" s="12">
         <f>basic_price!V33+tax_layer!V33+export_tax!V33</f>
@@ -18059,7 +18096,7 @@
       </c>
       <c r="AC33" s="12">
         <f>basic_price!AC33+tax_layer!AC33+export_tax!AC33</f>
-        <v>1310461.3520444911</v>
+        <v>1308238.0074955034</v>
       </c>
       <c r="AD33" s="12">
         <f>basic_price!AD33+tax_layer!AD33+export_tax!AD33</f>
@@ -18090,7 +18127,7 @@
       <c r="AN33" s="31"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -18198,7 +18235,7 @@
       </c>
       <c r="AC34" s="12">
         <f>basic_price!AC34+tax_layer!AC34+export_tax!AC34</f>
-        <v>2590414.0752308122</v>
+        <v>2589081.9285639026</v>
       </c>
       <c r="AD34" s="12">
         <f>basic_price!AD34+tax_layer!AD34+export_tax!AD34</f>
@@ -18229,7 +18266,7 @@
       <c r="AN34" s="31"/>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="3" t="s">
         <v>11</v>
       </c>
@@ -18368,7 +18405,7 @@
       <c r="AN35" s="31"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -18460,7 +18497,7 @@
       </c>
       <c r="Y36" s="12">
         <f>basic_price!Y36+tax_layer!Y36+export_tax!Y36</f>
-        <v>129953.17547229752</v>
+        <v>126809.5408523856</v>
       </c>
       <c r="Z36" s="12">
         <f>basic_price!Z36+tax_layer!Z36+export_tax!Z36</f>
@@ -18488,7 +18525,7 @@
       </c>
       <c r="AF36" s="12">
         <f>basic_price!AF36+tax_layer!AF36+export_tax!AF36</f>
-        <v>1711609.54427642</v>
+        <v>1714753.1788963322</v>
       </c>
       <c r="AG36" s="12">
         <f>basic_price!AG36+tax_layer!AG36+export_tax!AG36</f>
@@ -18507,7 +18544,7 @@
       <c r="AN36" s="31"/>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
@@ -18646,7 +18683,7 @@
       <c r="AN37" s="31"/>
     </row>
     <row r="38" spans="1:40" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
+      <c r="A38" s="48"/>
       <c r="B38" s="3" t="s">
         <v>28</v>
       </c>
@@ -18785,7 +18822,7 @@
       <c r="AN38" s="31"/>
     </row>
     <row r="39" spans="1:40" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="3" t="s">
         <v>28</v>
       </c>
@@ -18924,7 +18961,7 @@
       <c r="AN39" s="31"/>
     </row>
     <row r="40" spans="1:40" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="3" t="s">
         <v>28</v>
       </c>
@@ -19063,7 +19100,7 @@
       <c r="AN40" s="31"/>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
+      <c r="A41" s="49"/>
       <c r="B41" s="3" t="s">
         <v>28</v>
       </c>
@@ -19270,17 +19307,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="A16:A23"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A32:A41"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E4:L4"/>
     <mergeCell ref="M4:T4"/>
     <mergeCell ref="U4:AB4"/>
     <mergeCell ref="AC4:AI4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="A16:A23"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A32:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>